<commit_message>
Atualização de evolução do backlog
</commit_message>
<xml_diff>
--- a/Documentos/Demais Documentos do Projeto/Backlog do Produto - DW.xlsx
+++ b/Documentos/Demais Documentos do Projeto/Backlog do Produto - DW.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Demais Documentos do Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\10.10.228.100\mis_dados\04 - PROJETOS\DW\Data-Warehouse\Documentos\Demais Documentos do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010A51BC-102C-47C1-9261-52BDD5987D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF00F171-94B4-4912-B898-440AD15858DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="174">
   <si>
     <t>ETAPA</t>
   </si>
@@ -703,6 +703,9 @@
   </si>
   <si>
     <t>DBA / DA</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -4132,9 +4135,9 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999"/>
@@ -4273,7 +4276,9 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="7.5" customHeight="1">
-      <c r="D8" s="51"/>
+      <c r="D8" s="51" t="s">
+        <v>173</v>
+      </c>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
       <c r="G8" s="51"/>
@@ -5970,7 +5975,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H45 H10:H40</xm:sqref>
+          <xm:sqref>H10:H40 H45</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7232,7 +7237,7 @@
       </c>
       <c r="B1" s="61">
         <f ca="1">TODAY()+6</f>
-        <v>45501</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7257,7 +7262,7 @@
       </c>
       <c r="B4">
         <f ca="1">B2-B1</f>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7266,7 +7271,7 @@
       </c>
       <c r="B5" s="64">
         <f ca="1">B4-B3</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7283,7 +7288,7 @@
       </c>
       <c r="B7" s="62">
         <f ca="1">B5/B6</f>
-        <v>1.1538461538461537</v>
+        <v>1.0769230769230769</v>
       </c>
     </row>
     <row r="9" spans="1:2">

</xml_diff>

<commit_message>
Novos Arquivos e Querys
</commit_message>
<xml_diff>
--- a/Documentos/Demais Documentos do Projeto/Backlog do Produto - DW.xlsx
+++ b/Documentos/Demais Documentos do Projeto/Backlog do Produto - DW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\04 - PROJETOS\DW\Data-Warehouse\Documentos\Demais Documentos do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04255872-5E4B-49D9-99F5-8BDEB628CEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C7956F-C89F-401F-9D48-52D65C3E4DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,7 +717,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="dd/mm\ \-\ ddd"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2639,7 +2639,7 @@
       <selection pane="bottomLeft" activeCell="J12" sqref="I12:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="0.6640625" style="32" customWidth="1"/>
     <col min="3" max="3" width="0.5546875" style="51" customWidth="1"/>
@@ -2661,7 +2661,7 @@
     <col min="19" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="4.3499999999999996" customHeight="1">
+    <row r="1" spans="1:20" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D1" s="74" t="s">
         <v>115</v>
       </c>
@@ -2679,7 +2679,7 @@
       <c r="P1" s="52"/>
       <c r="Q1" s="52"/>
     </row>
-    <row r="2" spans="1:20" ht="3.15" customHeight="1">
+    <row r="2" spans="1:20" ht="3.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D2" s="74"/>
       <c r="E2" s="74"/>
       <c r="F2" s="74"/>
@@ -2695,7 +2695,7 @@
       <c r="P2" s="52"/>
       <c r="Q2" s="52"/>
     </row>
-    <row r="3" spans="1:20" ht="3.15" customHeight="1">
+    <row r="3" spans="1:20" ht="3.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
       <c r="F3" s="74"/>
@@ -2709,7 +2709,7 @@
       <c r="N3" s="74"/>
       <c r="O3" s="74"/>
     </row>
-    <row r="4" spans="1:20" ht="3.15" customHeight="1">
+    <row r="4" spans="1:20" ht="3.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="74"/>
       <c r="E4" s="74"/>
       <c r="F4" s="74"/>
@@ -2723,7 +2723,7 @@
       <c r="N4" s="74"/>
       <c r="O4" s="74"/>
     </row>
-    <row r="5" spans="1:20" ht="6.6" customHeight="1">
+    <row r="5" spans="1:20" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="74"/>
       <c r="E5" s="74"/>
       <c r="F5" s="74"/>
@@ -2737,7 +2737,7 @@
       <c r="N5" s="74"/>
       <c r="O5" s="74"/>
     </row>
-    <row r="6" spans="1:20" ht="7.2" customHeight="1">
+    <row r="6" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="74"/>
       <c r="E6" s="74"/>
       <c r="F6" s="74"/>
@@ -2754,7 +2754,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="51" customFormat="1" ht="14.4" customHeight="1">
+    <row r="7" spans="1:20" s="51" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="D7" s="74"/>
@@ -2773,7 +2773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="7.5" customHeight="1">
+    <row r="8" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
@@ -2789,7 +2789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>35</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="58">
         <f t="shared" ref="A10" si="0">IF(H10="-",0,1)</f>
         <v>1</v>
@@ -2884,7 +2884,7 @@
       <c r="Q10" s="25"/>
       <c r="T10" s="59"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="58">
         <f t="shared" ref="A11:A32" si="1">IF(H11="-",0,1)</f>
         <v>1</v>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="T11" s="59"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -2980,7 +2980,7 @@
       </c>
       <c r="T12" s="59"/>
     </row>
-    <row r="13" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="13" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="T13" s="59"/>
     </row>
-    <row r="14" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="14" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="T14" s="59"/>
     </row>
-    <row r="15" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="15" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="58">
         <f t="shared" ref="A15:A28" si="4">IF(H15="-",0,1)</f>
         <v>1</v>
@@ -3121,7 +3121,7 @@
       <c r="P15" s="25"/>
       <c r="T15" s="59"/>
     </row>
-    <row r="16" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="16" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3167,7 +3167,7 @@
       <c r="P16" s="25"/>
       <c r="T16" s="59"/>
     </row>
-    <row r="17" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="17" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3213,7 +3213,7 @@
       <c r="P17" s="25"/>
       <c r="T17" s="59"/>
     </row>
-    <row r="18" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="18" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3259,7 +3259,7 @@
       <c r="P18" s="25"/>
       <c r="T18" s="59"/>
     </row>
-    <row r="19" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="19" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3305,7 +3305,7 @@
       <c r="P19" s="25"/>
       <c r="T19" s="59"/>
     </row>
-    <row r="20" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="20" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3350,7 +3350,7 @@
       <c r="Q20" s="41"/>
       <c r="T20" s="59"/>
     </row>
-    <row r="21" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="21" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3397,7 +3397,7 @@
       <c r="Q21" s="41"/>
       <c r="T21" s="59"/>
     </row>
-    <row r="22" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="22" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3444,7 +3444,7 @@
       <c r="Q22" s="41"/>
       <c r="T22" s="59"/>
     </row>
-    <row r="23" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="23" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3491,7 +3491,7 @@
       <c r="Q23" s="41"/>
       <c r="T23" s="59"/>
     </row>
-    <row r="24" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="24" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3538,7 +3538,7 @@
       <c r="Q24" s="41"/>
       <c r="T24" s="59"/>
     </row>
-    <row r="25" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="25" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3585,7 +3585,7 @@
       <c r="Q25" s="41"/>
       <c r="T25" s="59"/>
     </row>
-    <row r="26" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="26" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3632,7 +3632,7 @@
       <c r="Q26" s="41"/>
       <c r="T26" s="59"/>
     </row>
-    <row r="27" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="27" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3679,7 +3679,7 @@
       <c r="Q27" s="41"/>
       <c r="T27" s="59"/>
     </row>
-    <row r="28" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="28" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="58">
         <f t="shared" si="4"/>
         <v>1</v>
@@ -3726,7 +3726,7 @@
       <c r="Q28" s="41"/>
       <c r="T28" s="59"/>
     </row>
-    <row r="29" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="29" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3773,7 +3773,7 @@
       <c r="Q29" s="41"/>
       <c r="T29" s="59"/>
     </row>
-    <row r="30" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="30" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3819,7 +3819,7 @@
       <c r="P30" s="59"/>
       <c r="T30" s="59"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3865,7 +3865,7 @@
       <c r="P31" s="59"/>
       <c r="T31" s="59"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="58">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -3911,7 +3911,7 @@
       <c r="P32" s="59"/>
       <c r="T32" s="59"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="57"/>
       <c r="B33" s="57"/>
       <c r="C33" s="53"/>
@@ -3919,7 +3919,7 @@
       <c r="P33" s="59"/>
       <c r="T33" s="59"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="57"/>
       <c r="B34" s="57"/>
       <c r="C34" s="53"/>
@@ -3927,7 +3927,7 @@
       <c r="P34" s="42"/>
       <c r="T34" s="59"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="57"/>
       <c r="B35" s="57"/>
       <c r="C35" s="53"/>
@@ -3935,7 +3935,7 @@
       <c r="P35" s="42"/>
       <c r="T35" s="59"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="57"/>
       <c r="B36" s="57"/>
       <c r="C36" s="53"/>
@@ -3943,7 +3943,7 @@
       <c r="P36" s="42"/>
       <c r="T36" s="59"/>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="57"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
@@ -3953,7 +3953,7 @@
       <c r="P37" s="42"/>
       <c r="T37" s="59"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="57"/>
       <c r="G38" s="30"/>
       <c r="K38" s="30"/>
@@ -3968,7 +3968,7 @@
       </c>
       <c r="T38" s="59"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="57"/>
       <c r="G39" s="30"/>
       <c r="K39" s="30"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="T39" s="59"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="57">
         <f>IF(H29="-",0,1)</f>
         <v>1</v>
@@ -3998,7 +3998,7 @@
       </c>
       <c r="T40" s="59"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="57">
         <f>IF(H30="-",0,1)</f>
         <v>1</v>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="T41" s="59"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="57">
         <f>IF(H31="-",0,1)</f>
         <v>1</v>
@@ -4028,7 +4028,7 @@
       </c>
       <c r="T42" s="59"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="57">
         <f>IF(H32="-",0,1)</f>
         <v>1</v>
@@ -4135,12 +4135,12 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5546875" style="32" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3.5546875" style="32" hidden="1" customWidth="1"/>
@@ -4163,7 +4163,7 @@
     <col min="19" max="16384" width="9.109375" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="4.3499999999999996" customHeight="1">
+    <row r="1" spans="1:20" ht="4.3499999999999996" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D1" s="74" t="s">
         <v>115</v>
       </c>
@@ -4181,7 +4181,7 @@
       <c r="P1" s="52"/>
       <c r="Q1" s="52"/>
     </row>
-    <row r="2" spans="1:20" ht="3.15" customHeight="1">
+    <row r="2" spans="1:20" ht="3.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="D2" s="74"/>
       <c r="E2" s="74"/>
       <c r="F2" s="74"/>
@@ -4197,7 +4197,7 @@
       <c r="P2" s="52"/>
       <c r="Q2" s="52"/>
     </row>
-    <row r="3" spans="1:20" ht="3.15" customHeight="1">
+    <row r="3" spans="1:20" ht="3.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="74"/>
       <c r="E3" s="74"/>
       <c r="F3" s="74"/>
@@ -4211,7 +4211,7 @@
       <c r="N3" s="74"/>
       <c r="O3" s="74"/>
     </row>
-    <row r="4" spans="1:20" ht="3.15" customHeight="1">
+    <row r="4" spans="1:20" ht="3.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="74"/>
       <c r="E4" s="74"/>
       <c r="F4" s="74"/>
@@ -4225,7 +4225,7 @@
       <c r="N4" s="74"/>
       <c r="O4" s="74"/>
     </row>
-    <row r="5" spans="1:20" ht="6.6" customHeight="1">
+    <row r="5" spans="1:20" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="74"/>
       <c r="E5" s="74"/>
       <c r="F5" s="74"/>
@@ -4239,7 +4239,7 @@
       <c r="N5" s="74"/>
       <c r="O5" s="74"/>
     </row>
-    <row r="6" spans="1:20" ht="7.2" customHeight="1">
+    <row r="6" spans="1:20" ht="7.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="74"/>
       <c r="E6" s="74"/>
       <c r="F6" s="74"/>
@@ -4256,7 +4256,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="51" customFormat="1" ht="14.4" customHeight="1">
+    <row r="7" spans="1:20" s="51" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="D7" s="74"/>
@@ -4275,7 +4275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="7.5" customHeight="1">
+    <row r="8" spans="1:20" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D8" s="51" t="s">
         <v>173</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>35</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="58">
         <f t="shared" ref="A10:A40" si="0">IF(H10="-",0,1)</f>
         <v>1</v>
@@ -4389,7 +4389,7 @@
       <c r="Q10" s="25"/>
       <c r="T10" s="59"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4440,7 +4440,7 @@
       </c>
       <c r="T11" s="59"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="T12" s="59"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4531,7 +4531,7 @@
       <c r="P13" s="25"/>
       <c r="T13" s="59"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4575,7 +4575,7 @@
       <c r="P14" s="25"/>
       <c r="T14" s="59"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4619,7 +4619,7 @@
       <c r="P15" s="25"/>
       <c r="T15" s="59"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4663,7 +4663,7 @@
       <c r="P16" s="25"/>
       <c r="T16" s="59"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4707,7 +4707,7 @@
       <c r="P17" s="25"/>
       <c r="T17" s="59"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4751,14 +4751,14 @@
       <c r="P18" s="25"/>
       <c r="T18" s="59"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B19" s="58">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C19" s="53"/>
       <c r="D19" s="26" t="s">
@@ -4774,7 +4774,7 @@
         <v>160</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I19" s="28" t="s">
         <v>171</v>
@@ -4795,14 +4795,14 @@
       <c r="P19" s="25"/>
       <c r="T19" s="59"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B20" s="58">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C20" s="53"/>
       <c r="D20" s="26" t="s">
@@ -4818,7 +4818,7 @@
         <v>161</v>
       </c>
       <c r="H20" s="27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I20" s="28" t="s">
         <v>171</v>
@@ -4839,7 +4839,7 @@
       <c r="P20" s="25"/>
       <c r="T20" s="59"/>
     </row>
-    <row r="21" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="21" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4887,14 +4887,14 @@
       </c>
       <c r="T21" s="59"/>
     </row>
-    <row r="22" spans="1:20" ht="10.8" customHeight="1">
+    <row r="22" spans="1:20" ht="10.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B22" s="58">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="53"/>
       <c r="D22" s="65" t="s">
@@ -4909,8 +4909,8 @@
       <c r="G22" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="68" t="s">
-        <v>5</v>
+      <c r="H22" s="27" t="s">
+        <v>3</v>
       </c>
       <c r="I22" s="69" t="s">
         <v>172</v>
@@ -4932,11 +4932,11 @@
       <c r="P22" s="25"/>
       <c r="Q22" s="32">
         <f>COUNTIF(Q9,H:H)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T22" s="59"/>
     </row>
-    <row r="23" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="23" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -4982,7 +4982,7 @@
       <c r="P23" s="25"/>
       <c r="T23" s="59"/>
     </row>
-    <row r="24" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="24" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5028,7 +5028,7 @@
       <c r="P24" s="25"/>
       <c r="T24" s="59"/>
     </row>
-    <row r="25" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="25" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5074,14 +5074,14 @@
       <c r="P25" s="25"/>
       <c r="T25" s="59"/>
     </row>
-    <row r="26" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="26" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B26" s="58">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C26" s="53"/>
       <c r="D26" s="26" t="s">
@@ -5097,7 +5097,7 @@
         <v>132</v>
       </c>
       <c r="H26" s="27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I26" s="28" t="s">
         <v>171</v>
@@ -5120,14 +5120,14 @@
       <c r="P26" s="25"/>
       <c r="T26" s="59"/>
     </row>
-    <row r="27" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="27" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B27" s="58">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="53"/>
       <c r="D27" s="26" t="s">
@@ -5143,7 +5143,7 @@
         <v>137</v>
       </c>
       <c r="H27" s="27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I27" s="28" t="s">
         <v>171</v>
@@ -5166,14 +5166,14 @@
       <c r="P27" s="25"/>
       <c r="T27" s="59"/>
     </row>
-    <row r="28" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="28" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B28" s="58">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C28" s="53"/>
       <c r="D28" s="65" t="s">
@@ -5188,8 +5188,8 @@
       <c r="G28" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="H28" s="68" t="s">
-        <v>5</v>
+      <c r="H28" s="27" t="s">
+        <v>4</v>
       </c>
       <c r="I28" s="69" t="s">
         <v>172</v>
@@ -5213,14 +5213,14 @@
       <c r="Q28" s="41"/>
       <c r="T28" s="59"/>
     </row>
-    <row r="29" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="29" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B29" s="58">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C29" s="53"/>
       <c r="D29" s="26" t="s">
@@ -5236,7 +5236,7 @@
         <v>128</v>
       </c>
       <c r="H29" s="27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" s="28" t="s">
         <v>171</v>
@@ -5260,7 +5260,7 @@
       <c r="Q29" s="41"/>
       <c r="T29" s="59"/>
     </row>
-    <row r="30" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="30" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5307,7 +5307,7 @@
       <c r="Q30" s="41"/>
       <c r="T30" s="59"/>
     </row>
-    <row r="31" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="31" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5354,7 +5354,7 @@
       <c r="Q31" s="41"/>
       <c r="T31" s="59"/>
     </row>
-    <row r="32" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="32" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5401,7 +5401,7 @@
       <c r="Q32" s="41"/>
       <c r="T32" s="59"/>
     </row>
-    <row r="33" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="33" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5448,7 +5448,7 @@
       <c r="Q33" s="41"/>
       <c r="T33" s="59"/>
     </row>
-    <row r="34" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="34" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5495,7 +5495,7 @@
       <c r="Q34" s="41"/>
       <c r="T34" s="59"/>
     </row>
-    <row r="35" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="35" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5542,7 +5542,7 @@
       <c r="Q35" s="41"/>
       <c r="T35" s="59"/>
     </row>
-    <row r="36" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="36" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5589,7 +5589,7 @@
       <c r="Q36" s="41"/>
       <c r="T36" s="59"/>
     </row>
-    <row r="37" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="37" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5636,7 +5636,7 @@
       <c r="Q37" s="41"/>
       <c r="T37" s="59"/>
     </row>
-    <row r="38" spans="1:20" ht="10.199999999999999" customHeight="1">
+    <row r="38" spans="1:20" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5682,7 +5682,7 @@
       <c r="P38" s="59"/>
       <c r="T38" s="59"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5728,7 +5728,7 @@
       <c r="P39" s="59"/>
       <c r="T39" s="59"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="58">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -5774,7 +5774,7 @@
       <c r="P40" s="59"/>
       <c r="T40" s="59"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="57"/>
       <c r="B41" s="57"/>
       <c r="C41" s="53"/>
@@ -5782,7 +5782,7 @@
       <c r="P41" s="59"/>
       <c r="T41" s="59"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="57"/>
       <c r="B42" s="57"/>
       <c r="C42" s="53"/>
@@ -5790,7 +5790,7 @@
       <c r="P42" s="42"/>
       <c r="T42" s="59"/>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="57"/>
       <c r="B43" s="57"/>
       <c r="C43" s="53"/>
@@ -5798,7 +5798,7 @@
       <c r="P43" s="42"/>
       <c r="T43" s="59"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="57"/>
       <c r="B44" s="57"/>
       <c r="C44" s="53"/>
@@ -5806,7 +5806,7 @@
       <c r="P44" s="42"/>
       <c r="T44" s="59"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="57"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
@@ -5816,7 +5816,7 @@
       <c r="P45" s="42"/>
       <c r="T45" s="59"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="57"/>
       <c r="G46" s="30"/>
       <c r="K46" s="30"/>
@@ -5831,7 +5831,7 @@
       </c>
       <c r="T46" s="59"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="57"/>
       <c r="G47" s="30"/>
       <c r="K47" s="30"/>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="T47" s="59"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="57">
         <f>IF(H37="-",0,1)</f>
         <v>1</v>
@@ -5861,7 +5861,7 @@
       </c>
       <c r="T48" s="59"/>
     </row>
-    <row r="49" spans="1:20">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="57">
         <f>IF(H38="-",0,1)</f>
         <v>1</v>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="T49" s="59"/>
     </row>
-    <row r="50" spans="1:20">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="57">
         <f>IF(H39="-",0,1)</f>
         <v>1</v>
@@ -5891,7 +5891,7 @@
       </c>
       <c r="T50" s="59"/>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="57">
         <f>IF(H40="-",0,1)</f>
         <v>1</v>
@@ -5975,7 +5975,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H10:H40 H45</xm:sqref>
+          <xm:sqref>H45 H10:H40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -6001,20 +6001,20 @@
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="5.0999999999999996" customHeight="1"/>
-    <row r="2" ht="5.0999999999999996" customHeight="1"/>
-    <row r="30" spans="8:8">
+    <row r="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>43299</v>
       </c>
     </row>
-    <row r="31" spans="8:8">
+    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H31">
         <v>43312</v>
       </c>
@@ -6036,7 +6036,7 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.109375" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="3.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.5546875" style="14" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3.21875" style="14" hidden="1" customWidth="1"/>
@@ -6052,7 +6052,7 @@
     <col min="18" max="16384" width="3.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="6" customHeight="1">
+    <row r="1" spans="1:17" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1">
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
@@ -6083,7 +6083,7 @@
       <c r="P2" s="77"/>
       <c r="Q2" s="77"/>
     </row>
-    <row r="3" spans="1:17" ht="22.65" customHeight="1">
+    <row r="3" spans="1:17" ht="22.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>8</v>
       </c>
@@ -6101,7 +6101,7 @@
       <c r="P3" s="77"/>
       <c r="Q3" s="77"/>
     </row>
-    <row r="4" spans="1:17" s="14" customFormat="1" ht="17.399999999999999">
+    <row r="4" spans="1:17" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.35">
       <c r="E4" s="13">
         <v>1E-3</v>
       </c>
@@ -6138,7 +6138,7 @@
       <c r="P4" s="40"/>
       <c r="Q4" s="40"/>
     </row>
-    <row r="5" spans="1:17" ht="18.899999999999999" customHeight="1">
+    <row r="5" spans="1:17" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" s="24" t="s">
         <v>6</v>
       </c>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="Q5" s="75"/>
     </row>
-    <row r="6" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="6" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="60">
         <f>SUMIFS(Backlog!$A:$A,Backlog!$D:$D,sintético!P6)</f>
@@ -6185,12 +6185,12 @@
       </c>
       <c r="C6" s="60">
         <f>SUMIF(Backlog!$D:$D,sintético!P6,Backlog!$B:$B)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="11">
         <f t="shared" ref="E6:E10" si="0">C6/B6</f>
-        <v>0.90909090909090906</v>
+        <v>1</v>
       </c>
       <c r="F6" s="39" t="str">
         <f>IF(AND($E6&gt;$E$4,$E6&lt;F$4),"DENTRO",IF($E6&gt;=F$4,"OK","FORA"))</f>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="O6" s="39" t="str">
         <f t="shared" si="2"/>
-        <v>DENTRO</v>
+        <v>OK</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>103</v>
@@ -6239,7 +6239,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="60">
         <f>SUMIFS(Backlog!$A:$A,Backlog!$D:$D,sintético!P7)</f>
@@ -6247,12 +6247,12 @@
       </c>
       <c r="C7" s="60">
         <f>SUMIF(Backlog!$D:$D,sintético!P7,Backlog!$B:$B)</f>
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>0.5714285714285714</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="F7" s="22" t="str">
         <f t="shared" ref="F7:F10" si="3">IF(AND($E7&gt;$E$4,$E7&lt;F$4),"DENTRO",IF($E7&gt;=F$4,"OK","FORA"))</f>
@@ -6276,23 +6276,23 @@
       </c>
       <c r="K7" s="22" t="str">
         <f t="shared" si="2"/>
-        <v>DENTRO</v>
+        <v>OK</v>
       </c>
       <c r="L7" s="22" t="str">
         <f>IF(AND(K7="OK",$E7&lt;L$4,$E7&gt;K$4),"DENTRO",IF($E7&gt;=L$4,"OK","FORA"))</f>
-        <v>FORA</v>
+        <v>OK</v>
       </c>
       <c r="M7" s="22" t="str">
         <f>IF(AND(L7="OK",$E7&lt;M$4,$E7&gt;L$4),"DENTRO",IF($E7&gt;=M$4,"OK","FORA"))</f>
-        <v>FORA</v>
+        <v>OK</v>
       </c>
       <c r="N7" s="22" t="str">
         <f t="shared" si="2"/>
-        <v>FORA</v>
+        <v>OK</v>
       </c>
       <c r="O7" s="22" t="str">
         <f t="shared" si="2"/>
-        <v>FORA</v>
+        <v>DENTRO</v>
       </c>
       <c r="P7" s="12" t="s">
         <v>104</v>
@@ -6301,7 +6301,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="60">
         <f>SUMIFS(Backlog!$A:$A,Backlog!$D:$D,sintético!P8)</f>
@@ -6309,20 +6309,20 @@
       </c>
       <c r="C8" s="60">
         <f>SUMIF(Backlog!$D:$D,sintético!P8,Backlog!$B:$B)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F8" s="22" t="str">
         <f t="shared" si="3"/>
-        <v>FORA</v>
+        <v>OK</v>
       </c>
       <c r="G8" s="22" t="str">
         <f t="shared" si="1"/>
-        <v>FORA</v>
+        <v>DENTRO</v>
       </c>
       <c r="H8" s="22" t="str">
         <f t="shared" si="2"/>
@@ -6363,7 +6363,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="60">
         <f>SUMIFS(Backlog!$A:$A,Backlog!$D:$D,sintético!P9)</f>
@@ -6425,7 +6425,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="60">
         <f>SUMIFS(Backlog!$A:$A,Backlog!$D:$D,sintético!P10)</f>
@@ -6487,7 +6487,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="14">
         <f>SUMIFS(Backlog_old!$A:$A,Backlog_old!$D:$D,sintético!#REF!)</f>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="D11" s="14"/>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14">
         <f>SUMIFS(Backlog_old!$A:$A,Backlog_old!$D:$D,sintético!#REF!)</f>
@@ -6511,7 +6511,7 @@
       </c>
       <c r="D12" s="14"/>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14">
         <f>SUMIFS(Backlog_old!$A:$A,Backlog_old!$D:$D,sintético!#REF!)</f>
@@ -6523,7 +6523,7 @@
       </c>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -6540,7 +6540,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -6557,7 +6557,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -6574,7 +6574,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="17" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -6591,7 +6591,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="18" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
@@ -6608,7 +6608,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="19" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -6625,7 +6625,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="20" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -6642,7 +6642,7 @@
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -6661,7 +6661,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="22" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -6680,7 +6680,7 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="23" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -6699,7 +6699,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="24" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -6718,7 +6718,7 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="25" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -6737,7 +6737,7 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="26" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -6756,7 +6756,7 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="27" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
@@ -6775,7 +6775,7 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="28" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -6794,7 +6794,7 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="29" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -6813,7 +6813,7 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="30" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14"/>
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
@@ -6832,7 +6832,7 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="31" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="14"/>
@@ -6851,7 +6851,7 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="32" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -6870,7 +6870,7 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="33" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="14"/>
@@ -6889,7 +6889,7 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="34" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -6908,7 +6908,7 @@
       <c r="P34" s="5"/>
       <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="35" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="14"/>
@@ -6927,7 +6927,7 @@
       <c r="P35" s="5"/>
       <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="36" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -6946,7 +6946,7 @@
       <c r="P36" s="5"/>
       <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="37" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="14"/>
       <c r="C37" s="14"/>
@@ -6965,7 +6965,7 @@
       <c r="P37" s="5"/>
       <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="38" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="14"/>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -6984,7 +6984,7 @@
       <c r="P38" s="5"/>
       <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="39" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -7003,7 +7003,7 @@
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="40" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14"/>
       <c r="B40" s="14"/>
       <c r="C40" s="14"/>
@@ -7022,7 +7022,7 @@
       <c r="P40" s="5"/>
       <c r="Q40" s="5"/>
     </row>
-    <row r="41" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="41" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="14"/>
@@ -7041,7 +7041,7 @@
       <c r="P41" s="5"/>
       <c r="Q41" s="5"/>
     </row>
-    <row r="42" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="42" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="14"/>
@@ -7060,7 +7060,7 @@
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="43" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="14"/>
@@ -7079,7 +7079,7 @@
       <c r="P43" s="5"/>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="44" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -7098,7 +7098,7 @@
       <c r="P44" s="5"/>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="45" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="14"/>
@@ -7117,7 +7117,7 @@
       <c r="P45" s="5"/>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="46" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -7136,7 +7136,7 @@
       <c r="P46" s="8"/>
       <c r="Q46" s="8"/>
     </row>
-    <row r="47" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="47" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -7155,7 +7155,7 @@
       <c r="P47" s="9"/>
       <c r="Q47" s="9"/>
     </row>
-    <row r="48" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="48" spans="1:17" s="1" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -7172,7 +7172,7 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
     </row>
-    <row r="49" spans="1:17" s="9" customFormat="1" ht="18.899999999999999" customHeight="1">
+    <row r="49" spans="1:17" s="9" customFormat="1" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -7225,22 +7225,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>144</v>
       </c>
       <c r="B1" s="61">
         <f ca="1">TODAY()+6</f>
-        <v>45505</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>45510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>45534</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>146</v>
       </c>
@@ -7256,25 +7256,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>147</v>
       </c>
       <c r="B4">
         <f ca="1">B2-B1</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>148</v>
       </c>
       <c r="B5" s="64">
         <f ca="1">B4-B3</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -7282,16 +7282,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>150</v>
       </c>
       <c r="B7" s="62">
         <f ca="1">B5/B6</f>
-        <v>0.84615384615384615</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>0.46153846153846156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -7300,7 +7300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -7331,14 +7331,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="str">
         <f>Backlog_old!F10</f>
         <v>Design e Modelagem de Dados</v>
@@ -7356,7 +7356,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="str">
         <f>Backlog_old!F13</f>
         <v>Desenvolvimento e Implementação</v>
@@ -7374,7 +7374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="str">
         <f>Backlog_old!F31</f>
         <v>Implantação</v>
@@ -7392,31 +7392,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="38"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="31"/>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="38"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="31"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="38"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="31"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="38"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="31"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
@@ -7446,7 +7446,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -7454,7 +7454,7 @@
     <col min="4" max="4" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="43" t="s">
         <v>40</v>
       </c>
@@ -7464,19 +7464,19 @@
       <c r="C1" s="45"/>
       <c r="D1" s="46"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="46"/>
       <c r="B2" s="47"/>
       <c r="C2" s="45"/>
       <c r="D2" s="46"/>
     </row>
-    <row r="3" spans="1:4" ht="15.6">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="45"/>
       <c r="D3" s="46"/>
     </row>
-    <row r="4" spans="1:4" ht="15.6">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="46"/>
       <c r="B4" s="47"/>
       <c r="C4" s="48" t="s">
@@ -7486,7 +7486,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
       <c r="C5" s="45" t="s">
@@ -7496,13 +7496,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="46"/>
       <c r="B6" s="47"/>
       <c r="C6" s="50"/>
       <c r="D6" s="50"/>
     </row>
-    <row r="7" spans="1:4" ht="15.6">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="46"/>
       <c r="B7" s="47"/>
       <c r="C7" s="48" t="s">
@@ -7512,7 +7512,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="46"/>
       <c r="B8" s="47"/>
       <c r="C8" s="45" t="str">
@@ -7523,13 +7523,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="46"/>
       <c r="B9" s="47"/>
       <c r="C9" s="50"/>
       <c r="D9" s="50"/>
     </row>
-    <row r="10" spans="1:4" ht="15.6">
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="46"/>
       <c r="B10" s="47"/>
       <c r="C10" s="48" t="s">
@@ -7539,7 +7539,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6">
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="46"/>
       <c r="B11" s="47"/>
       <c r="C11" s="45" t="s">
@@ -7549,25 +7549,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6">
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="46"/>
       <c r="B12" s="47"/>
       <c r="C12" s="46"/>
       <c r="D12" s="46"/>
     </row>
-    <row r="13" spans="1:4" ht="15.6">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="46"/>
       <c r="B13" s="47"/>
       <c r="C13" s="45"/>
       <c r="D13" s="46"/>
     </row>
-    <row r="14" spans="1:4" ht="15.6">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="46"/>
       <c r="B14" s="47"/>
       <c r="C14" s="45"/>
       <c r="D14" s="46"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="46"/>
       <c r="B15" s="46"/>
       <c r="C15" s="48" t="s">
@@ -7577,7 +7577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
         <v>48</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>50</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="46" t="s">
         <v>52</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="46" t="s">
         <v>54</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="46" t="s">
         <v>56</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="46" t="s">
         <v>56</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="46" t="s">
         <v>60</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="46"/>
       <c r="B23" s="46"/>
       <c r="C23" s="45"/>
@@ -7716,7 +7716,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
@@ -7726,7 +7726,7 @@
     <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>136002</v>
       </c>
@@ -7772,7 +7772,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>136002</v>
       </c>
@@ -7795,7 +7795,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>136002</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>136001</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>136001</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>136001</v>
       </c>
@@ -7900,7 +7900,7 @@
       <selection activeCell="B4" sqref="B4:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.5546875" customWidth="1"/>
     <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
@@ -7911,7 +7911,7 @@
     <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E1" s="16" t="s">
         <v>3</v>
       </c>
@@ -7928,12 +7928,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:11">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
         <v>0</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>9</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:11">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
@@ -7960,7 +7960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="2:11">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>11</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>12</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:11">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>13</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:11">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>14</v>
       </c>
@@ -7992,7 +7992,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:11">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>15</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>31</v>
       </c>
@@ -8008,14 +8008,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:11">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="18"/>
       <c r="C12" s="20"/>
     </row>
-    <row r="13" spans="2:11">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C13" s="20"/>
     </row>
-    <row r="14" spans="2:11">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C14" s="20"/>
     </row>
   </sheetData>

</xml_diff>